<commit_message>
Refactor cleanup script to delete report.xlsx for fresh creation by orchestrator; update memory.md documentation for clarity on swarm mode changes.
</commit_message>
<xml_diff>
--- a/.docs/report.xlsx
+++ b/.docs/report.xlsx
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,23 +31,13 @@
     </font>
     <font>
       <b val="1"/>
-      <color rgb="00db2777"/>
-      <sz val="18"/>
+      <sz val="16"/>
     </font>
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="14"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -56,17 +46,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00f9a8d4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00db2777"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00fce7f3"/>
+        <fgColor rgb="00E0E0E0"/>
       </patternFill>
     </fill>
   </fills>
@@ -82,17 +62,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -458,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,8 +439,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -480,182 +453,62 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Plan File</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(pending)</t>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Value</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Generated</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>(pending)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Total Tasks</t>
         </is>
       </c>
-      <c r="B8">
+      <c r="B4">
         <f>COUNTA(Tasks!A:A)-1</f>
         <v/>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Completed Tasks</t>
+        </is>
+      </c>
+      <c r="B5">
+        <f>COUNTIF(Tasks!C:C,"Done")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Total Waves</t>
         </is>
       </c>
-      <c r="B9">
-        <f>MAX(Tasks!B:B)</f>
+      <c r="B6">
+        <f>COUNTA(Waves!A:A)-1</f>
         <v/>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Completed Tasks</t>
-        </is>
-      </c>
-      <c r="B10">
-        <f>COUNTIF(Tasks!G:G,"Complete")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Failed Tasks</t>
-        </is>
-      </c>
-      <c r="B11">
-        <f>COUNTIF(Tasks!G:G,"Failed")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Running Tasks</t>
-        </is>
-      </c>
-      <c r="B12">
-        <f>COUNTIF(Tasks!G:G,"Running")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>Total Duration (min)</t>
-        </is>
-      </c>
-      <c r="B13">
-        <f>SUM(Tasks!F:F)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>Total Tokens</t>
-        </is>
-      </c>
-      <c r="B14">
-        <f>SUM(Tasks!I:I)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="inlineStr">
-        <is>
-          <t>Avg Context Window</t>
-        </is>
-      </c>
-      <c r="B15">
-        <f>IFERROR(AVERAGE(Tasks!J:J),0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5" t="inlineStr">
-        <is>
-          <t>Efficiency Metrics</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="inlineStr">
-        <is>
-          <t>Sequential Est. (min)</t>
-        </is>
-      </c>
-      <c r="B19">
-        <f>B8*5</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="inlineStr">
-        <is>
-          <t>Parallel Actual (min)</t>
-        </is>
-      </c>
-      <c r="B20">
-        <f>B13</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="inlineStr">
-        <is>
-          <t>Time Saved (%)</t>
-        </is>
-      </c>
-      <c r="B21">
-        <f>IF(B19&gt;0,(B19-B20)/B19*100,0)</f>
-        <v/>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Total Duration</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>(after run)</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A18:B18"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -668,7 +521,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -676,85 +529,49 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
-    <col width="30" customWidth="1" min="11" max="11"/>
-    <col width="15" customWidth="1" min="12" max="12"/>
-    <col width="40" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Task Name</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
-        <is>
-          <t>Wave</t>
-        </is>
-      </c>
-      <c r="C1" s="7" t="inlineStr">
-        <is>
-          <t>Agent ID</t>
-        </is>
-      </c>
-      <c r="D1" s="7" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="E1" s="7" t="inlineStr">
-        <is>
-          <t>End Time</t>
-        </is>
-      </c>
-      <c r="F1" s="7" t="inlineStr">
-        <is>
-          <t>Duration (min)</t>
-        </is>
-      </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Agent</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Tokens</t>
         </is>
       </c>
-      <c r="J1" s="7" t="inlineStr">
-        <is>
-          <t>Context Window</t>
-        </is>
-      </c>
-      <c r="K1" s="7" t="inlineStr">
-        <is>
-          <t>Files Changed</t>
-        </is>
-      </c>
-      <c r="L1" s="7" t="inlineStr">
-        <is>
-          <t>Commit Hash</t>
-        </is>
-      </c>
-      <c r="M1" s="7" t="inlineStr">
-        <is>
-          <t>Notes</t>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
         </is>
       </c>
     </row>
@@ -769,7 +586,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -777,119 +594,43 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
-        <is>
-          <t>Wave #</t>
-        </is>
-      </c>
-      <c r="B1" s="7" t="inlineStr">
-        <is>
-          <t>Task Count</t>
-        </is>
-      </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Wave</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Agents</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
-        <is>
-          <t>Duration (min)</t>
-        </is>
-      </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Status</t>
-        </is>
-      </c>
-      <c r="G1" s="7" t="inlineStr">
-        <is>
-          <t>Parallel Agents</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>COUNTIF(Tasks!B:B,0)</f>
-        <v/>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f>COUNTIF(Tasks!B:B,1)</f>
-        <v/>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <f>COUNTIF(Tasks!B:B,2)</f>
-        <v/>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <f>COUNTIF(Tasks!B:B,3)</f>
-        <v/>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <f>COUNTIF(Tasks!B:B,4)</f>
-        <v/>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Pending</t>
         </is>
       </c>
     </row>
@@ -904,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,66 +654,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="20" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="50" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
-        <is>
-          <t>Agent ID</t>
-        </is>
-      </c>
-      <c r="B1" s="7" t="inlineStr">
-        <is>
-          <t>Worktree Path</t>
-        </is>
-      </c>
-      <c r="C1" s="7" t="inlineStr">
-        <is>
-          <t>Task Assigned</t>
-        </is>
-      </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Agent Name</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Wave</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
-        <is>
-          <t>PID/Job Name</t>
-        </is>
-      </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Tokens</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Status</t>
-        </is>
-      </c>
-      <c r="G1" s="7" t="inlineStr">
-        <is>
-          <t>Started</t>
-        </is>
-      </c>
-      <c r="H1" s="7" t="inlineStr">
-        <is>
-          <t>Finished</t>
-        </is>
-      </c>
-      <c r="I1" s="7" t="inlineStr">
-        <is>
-          <t>Exit Code</t>
-        </is>
-      </c>
-      <c r="J1" s="7" t="inlineStr">
-        <is>
-          <t>Error Log</t>
         </is>
       </c>
     </row>
@@ -987,7 +704,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,31 +712,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
-        <is>
-          <t>Event Type</t>
-        </is>
-      </c>
-      <c r="C1" s="7" t="inlineStr">
-        <is>
-          <t>Agent/Wave</t>
-        </is>
-      </c>
-      <c r="D1" s="7" t="inlineStr">
-        <is>
-          <t>Description</t>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Details</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update memory.md to clarify implementation reference and modify report.xlsx
</commit_message>
<xml_diff>
--- a/.docs/report.xlsx
+++ b/.docs/report.xlsx
@@ -10,8 +10,9 @@
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Tasks" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Waves" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Agents" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Timeline" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Research" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Agents" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Timeline" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -51,8 +52,12 @@
       <b val="1"/>
       <color rgb="00DB2777"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -72,6 +77,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00F9A8D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005B21B6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009333EA"/>
       </patternFill>
     </fill>
   </fills>
@@ -101,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -114,6 +129,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -572,9 +594,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>Total Duration</t>
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>Agent Metrics</t>
         </is>
       </c>
       <c r="B8" s="6" t="inlineStr">
@@ -591,11 +613,11 @@
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>Tokens Used</t>
+          <t>Background CLI Agents</t>
         </is>
       </c>
       <c r="B9" s="4">
-        <f>SUM(Tasks!F:F)</f>
+        <f>COUNTIF(Agents!C:C,"Background CLI")</f>
         <v/>
       </c>
       <c r="C9" s="5" t="inlineStr">
@@ -607,17 +629,28 @@
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>Success Rate</t>
+          <t>Subagent Research Calls</t>
         </is>
       </c>
       <c r="B10" s="6">
-        <f>IF(B5&gt;0,ROUND(B6/B5*100,1)&amp;"%","N/A")</f>
+        <f>COUNTA(Research!A:A)-1</f>
         <v/>
       </c>
       <c r="C10" s="7" t="inlineStr">
         <is>
           <t>Completed/Total</t>
         </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Total Agent Operations</t>
+        </is>
+      </c>
+      <c r="B11">
+        <f>B9+B10</f>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -691,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -719,27 +752,32 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Duration</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Tokens</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
@@ -815,7 +853,78 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="12" t="inlineStr">
+        <is>
+          <t>Research ID</t>
+        </is>
+      </c>
+      <c r="B1" s="12" t="inlineStr">
+        <is>
+          <t>After Wave</t>
+        </is>
+      </c>
+      <c r="C1" s="12" t="inlineStr">
+        <is>
+          <t>Purpose</t>
+        </is>
+      </c>
+      <c r="D1" s="12" t="inlineStr">
+        <is>
+          <t>Findings Summary</t>
+        </is>
+      </c>
+      <c r="E1" s="12" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="F1" s="12" t="inlineStr">
+        <is>
+          <t>Tokens</t>
+        </is>
+      </c>
+      <c r="G1" s="12" t="inlineStr">
+        <is>
+          <t>Enriched Wave</t>
+        </is>
+      </c>
+      <c r="H1" s="12" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -843,27 +952,32 @@
           <t>Task</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Wave</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Worktree</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Duration</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Tokens</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -874,7 +988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>